<commit_message>
Changes to Lab 2
</commit_message>
<xml_diff>
--- a/02_assignments/data/homelessness_data.xlsx
+++ b/02_assignments/data/homelessness_data.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Teaching\regression\02_assignments\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4E9AE-D4E7-4F9B-B094-D7D8A1F284EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31BEC5A-9A1F-4123-A390-BCBEF6934448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homelessness" sheetId="1" r:id="rId1"/>
     <sheet name="Census Data" sheetId="2" r:id="rId2"/>
     <sheet name="Region" sheetId="4" r:id="rId3"/>
     <sheet name="Federal Aid" sheetId="5" r:id="rId4"/>
+    <sheet name="Cell Ref Practice" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="980">
   <si>
     <t>Alabama</t>
   </si>
@@ -2865,12 +2867,129 @@
   </si>
   <si>
     <t>total_homeless_pop</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Total Mileage</t>
+  </si>
+  <si>
+    <t>Total Owed</t>
+  </si>
+  <si>
+    <t>Reimbursement Rate</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Jan Rate</t>
+  </si>
+  <si>
+    <t>Feb Rate</t>
+  </si>
+  <si>
+    <t>March Rate</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Find Kelsey's ID #</t>
+  </si>
+  <si>
+    <t>Find the name of the person with ID# 34</t>
+  </si>
+  <si>
+    <t>Annie</t>
+  </si>
+  <si>
+    <t>MATCH</t>
+  </si>
+  <si>
+    <t>Brett</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Elaine</t>
+  </si>
+  <si>
+    <t>INDEX(MATCH())</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Hank</t>
+  </si>
+  <si>
+    <t>Ingrid</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Kelsey</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Nigel</t>
+  </si>
+  <si>
+    <t>Ophelia</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>Quincy</t>
+  </si>
+  <si>
+    <t>Randin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2880,15 +2999,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8CBEA7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2896,20 +3021,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8CBEA7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3187,7 +3408,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D52"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3780,7 +4001,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5926,7 +6147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A10EA4-A451-4601-8C42-7C149645B643}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -6357,7 +6578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09353E5-526F-4502-B5CF-27162637E468}">
   <dimension ref="A1:Y397"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
@@ -36902,4 +37123,378 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C026CDCB-4A17-4CDF-89A6-BFC41C7C660F}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C1" t="s">
+        <v>944</v>
+      </c>
+      <c r="D1" t="s">
+        <v>945</v>
+      </c>
+      <c r="E1" t="s">
+        <v>946</v>
+      </c>
+      <c r="F1" t="s">
+        <v>947</v>
+      </c>
+      <c r="H1" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>279</v>
+      </c>
+      <c r="D2">
+        <v>172</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>950</v>
+      </c>
+      <c r="B3">
+        <v>108</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>951</v>
+      </c>
+      <c r="B4">
+        <v>158</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>135</v>
+      </c>
+      <c r="H4" t="s">
+        <v>952</v>
+      </c>
+      <c r="I4" t="s">
+        <v>953</v>
+      </c>
+      <c r="J4" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>955</v>
+      </c>
+      <c r="B5">
+        <v>293</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>195</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>955</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EABC40-DD63-4D59-8291-97BDF819B054}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B1" t="s">
+        <v>883</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B2" s="7">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="E2" s="8" t="s">
+        <v>960</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>961</v>
+      </c>
+      <c r="B3" s="7">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>962</v>
+      </c>
+      <c r="B4" s="7">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="E4" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>964</v>
+      </c>
+      <c r="B5" s="7">
+        <v>43</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>965</v>
+      </c>
+      <c r="B6" s="7">
+        <v>95</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>967</v>
+      </c>
+      <c r="B7" s="7">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>968</v>
+      </c>
+      <c r="B8" s="7">
+        <v>88</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>969</v>
+      </c>
+      <c r="B9" s="7">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>970</v>
+      </c>
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>971</v>
+      </c>
+      <c r="B11" s="7">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>972</v>
+      </c>
+      <c r="B12" s="7">
+        <v>68</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>973</v>
+      </c>
+      <c r="B13" s="7">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>974</v>
+      </c>
+      <c r="B14" s="7">
+        <v>95</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>975</v>
+      </c>
+      <c r="B15" s="7">
+        <v>31</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>976</v>
+      </c>
+      <c r="B16" s="7">
+        <v>34</v>
+      </c>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>977</v>
+      </c>
+      <c r="B17" s="7">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>978</v>
+      </c>
+      <c r="B18" s="7">
+        <v>94</v>
+      </c>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>979</v>
+      </c>
+      <c r="B19" s="7">
+        <v>39</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>